<commit_message>
this is new commit
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="26">
   <si>
     <t>Tamil Nau, Chennai</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Please fill in this field.</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>

</xml_diff>